<commit_message>
- Se agrega el modelado de amenazas modificado - Se agrega el contenedor de servicios que hace el monitoreo al host - Se añade el manejo de bitácoras - Se añade el la actualización de la tabla con AJAX - Modificaciones a estilos de login, verificación de usuario y monitor
</commit_message>
<xml_diff>
--- a/modeladoAmenazas.xlsx
+++ b/modeladoAmenazas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porsc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Universidad\8vo Semestre\ProgramacionSegura\proyectoProgramSegura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D71622-71E9-4610-AA31-80BC777A355E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A94748-4F3E-492F-878B-5A78920B5504}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{040DBA77-213F-4200-AEDF-EE5D762F9109}"/>
+    <workbookView xWindow="16212" yWindow="-1668" windowWidth="23256" windowHeight="12576" xr2:uid="{040DBA77-213F-4200-AEDF-EE5D762F9109}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Tipo de elemento DFD</t>
   </si>
@@ -150,12 +150,6 @@
     <t xml:space="preserve">permisos para usuarios (T)              bitácoras de registro de actividades (R )  comunicación cifrada (I)      </t>
   </si>
   <si>
-    <t>connectServer</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>Almacenes: adminData 1.5 serverData 1.6                              Flujo de datos: enviarCredenciales(3.0 -&gt; 1.7 -&gt; 3.0), revisarCredenciales(1.7 -&gt; 1.5 -&gt; 1.7) Procesos: login 1.7</t>
   </si>
   <si>
@@ -171,22 +165,37 @@
     <t>Almacenes: adminData 1.5                             serverData 1.6                                                              Flujo de datos: enviarCredenciales(3.0 -&gt; 1.7 -&gt; 3.0), revisarCredenciales(1.7 -&gt; 1.5 -&gt; 1.7)                 Procesos: login 1.7</t>
   </si>
   <si>
-    <t>globalAdmin 1.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">serverAdmin 2.0 </t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
-    <t>Entidades externas: anonymous 3.0,            globalAdmin 1.0                                             serverAdmin 2.0                                                  Procesos: login 1.7</t>
-  </si>
-  <si>
     <t xml:space="preserve">R                         </t>
   </si>
   <si>
     <t>bitácoras de intentos (R )</t>
+  </si>
+  <si>
+    <t>Entidades externas: anonymous 3.0,                                                     serverAdmin 2.0                                                  Procesos: login 1.7</t>
+  </si>
+  <si>
+    <t>Con el módulo de login  se añadieron los parámetros para que registre que usuario intento realizar una conexión al sistema</t>
+  </si>
+  <si>
+    <t>Se utilizo una autenticación en conjunto con un bot en Telegram que envía un token a un chat donde se encuentra el usuario que desea acceder al sistema.</t>
+  </si>
+  <si>
+    <t>Para limitar intentos se ocupó un script desarrollado en clase donde por medio de la dirección IP de la cual se desea acceder al sistema se guarda como una variable que hace un conteo del número de intentos y después de rebasar el límite (en nuestro caso 5) es bloqueado por un espacio de tiempo. La validación de entradas y sanitización son hechas por defecto en Django y para las bitácoras de intentos, se impoto el módulo de login y en el archivo de views se agrega las partes en el código donde se necesita usar un log.</t>
+  </si>
+  <si>
+    <t>Se usaron certificados auto firmados por cuestiones prácticas sin embargo para un sistema en producción es recomendable tener certificados avalados por unas organizaciones acreditadas. Las bitácoras de intentos, se importó el módulo de login y en el archivo de views se agrega las partes en el código donde se necesita usar un log.</t>
+  </si>
+  <si>
+    <t>Los permisos son asignados por el administrador global desde la creación del mismo por medio del módulo auth, las bitácoras de registro también son proporcionados por el módulo auth que registra las actividades del administrador global, se implementó comunicacion por HTTPS</t>
+  </si>
+  <si>
+    <t>Por medio del módulo auth y funciones de cifrado se guardan las contraseñas cifradas en la base de datos, además de implementar comunicación con HTTPS con certificados auto firmados (no recomendable para un sistema en producción)</t>
   </si>
 </sst>
 </file>
@@ -228,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -242,6 +251,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,25 +569,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645491CC-57F8-45A5-B33B-9D0D702F60CE}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.88671875" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.88671875" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="70.140625" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" customWidth="1"/>
     <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -591,7 +603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -599,7 +611,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -607,7 +619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="173.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="173.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -615,8 +627,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="46.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="46.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -624,47 +636,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -672,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -685,8 +697,9 @@
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -694,71 +707,86 @@
         <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>26</v>
@@ -769,63 +797,46 @@
       <c r="D23" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>30</v>
+      <c r="E25" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>